<commit_message>
agenda 7 logboek update
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_jp.xlsx
+++ b/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_jp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Dag:</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Vrijdag: soft delete en update verbetert</t>
+  </si>
+  <si>
+    <t>Vrijdag: testen</t>
+  </si>
+  <si>
+    <t>Donderdag:  oplevering</t>
   </si>
 </sst>
 </file>
@@ -774,15 +780,36 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -792,14 +819,47 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,80 +867,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1169,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96:J96"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,11 +1185,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="3" spans="1:17" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
@@ -1242,11 +1248,11 @@
       <c r="J5" s="7">
         <v>2</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="O5" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="40"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="46"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
@@ -1274,11 +1280,11 @@
         <v>2</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="O6" s="47" t="s">
+      <c r="O6" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="49"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
@@ -1305,11 +1311,11 @@
       <c r="J7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="43"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
@@ -1336,11 +1342,11 @@
       <c r="J8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="41" t="s">
+      <c r="O8" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="43"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
@@ -1364,28 +1370,36 @@
         <v>2</v>
       </c>
       <c r="K9" s="8"/>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="43"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="7">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="O10" s="44" t="s">
+      <c r="O10" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="46"/>
+      <c r="P10" s="53"/>
+      <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C11" s="9" t="s">
@@ -1460,13 +1474,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B16" s="8"/>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="12">
         <f>SUM((D5,D6,D7,D8,D9,D10,D11,D12,E5,E6,E7,E8,E9,E10,E11,E12,F5,F6,F7,F8,F9,F10,F11,F12,G5,G6,G7,G8,G9,G10,G11,G12,H5,H6,H7,H8,H9,H10,H11,H12,I5,I6,I7,I8,I9,I10,I11,I12,J5,J6,J7,J8,J9,J10,J11,J12,D13,D14,E13,E14,F13,F14,G13,G14,H13,H14,I13,I14,J13,J14))</f>
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -1517,100 +1531,100 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="25"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="37"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="28"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
@@ -1641,100 +1655,100 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="31"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="25"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="25"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="14"/>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="14"/>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="25"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="25"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="28"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
@@ -1765,100 +1779,100 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="14"/>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="31"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="14"/>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="25"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="14"/>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="25"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="14"/>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="28"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="14"/>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="25"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="14"/>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="25"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="14"/>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="28"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
@@ -1889,100 +1903,100 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="11"/>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="31"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="25"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="31"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="25"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="31"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="37"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="28"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="25"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="31"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="25"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="31"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="28"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="35"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
@@ -2013,92 +2027,92 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="31"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="42"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="25"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30"/>
+      <c r="J57" s="31"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="25"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="31"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="37"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="28"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C60" s="23" t="s">
+      <c r="C60" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="25"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="31"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="24"/>
-      <c r="J61" s="25"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="31"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="28"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="35"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C63" s="21"/>
@@ -2123,88 +2137,88 @@
       <c r="J64" s="18"/>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="30"/>
-      <c r="I65" s="30"/>
-      <c r="J65" s="31"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="42"/>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="24"/>
-      <c r="J66" s="25"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="30"/>
+      <c r="J66" s="31"/>
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="24"/>
-      <c r="J67" s="25"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="30"/>
+      <c r="J67" s="31"/>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C68" s="57" t="s">
+      <c r="C68" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="37"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="28"/>
     </row>
     <row r="69" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
-      <c r="J69" s="25"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="31"/>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C70" s="23" t="s">
+      <c r="C70" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="25"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="30"/>
+      <c r="J70" s="31"/>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C71" s="26" t="s">
+      <c r="C71" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="28"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
+      <c r="H71" s="34"/>
+      <c r="I71" s="34"/>
+      <c r="J71" s="35"/>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C72" s="21"/>
@@ -2229,88 +2243,88 @@
       <c r="J73" s="18"/>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C74" s="58" t="s">
+      <c r="C74" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30"/>
-      <c r="J74" s="31"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="42"/>
     </row>
     <row r="75" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C75" s="56" t="s">
+      <c r="C75" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="24"/>
-      <c r="I75" s="24"/>
-      <c r="J75" s="25"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="31"/>
     </row>
     <row r="76" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C76" s="56" t="s">
+      <c r="C76" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="25"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="31"/>
     </row>
     <row r="77" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C77" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="37"/>
+      <c r="C77" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="27"/>
+      <c r="I77" s="27"/>
+      <c r="J77" s="28"/>
     </row>
     <row r="78" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C78" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="25"/>
+      <c r="C78" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="30"/>
+      <c r="G78" s="30"/>
+      <c r="H78" s="30"/>
+      <c r="I78" s="30"/>
+      <c r="J78" s="31"/>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="25"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="30"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="30"/>
+      <c r="J79" s="31"/>
     </row>
     <row r="80" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C80" s="26" t="s">
+      <c r="C80" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="28"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="34"/>
+      <c r="J80" s="35"/>
     </row>
     <row r="81" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C81" s="21"/>
@@ -2335,88 +2349,88 @@
       <c r="J82" s="18"/>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C83" s="50" t="s">
+      <c r="C83" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="51"/>
-      <c r="E83" s="51"/>
-      <c r="F83" s="51"/>
-      <c r="G83" s="51"/>
-      <c r="H83" s="51"/>
-      <c r="I83" s="51"/>
-      <c r="J83" s="52"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="38"/>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C84" s="53" t="s">
+      <c r="C84" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D84" s="54"/>
-      <c r="E84" s="54"/>
-      <c r="F84" s="54"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-      <c r="J84" s="55"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="25"/>
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C85" s="53" t="s">
+      <c r="C85" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D85" s="54"/>
-      <c r="E85" s="54"/>
-      <c r="F85" s="54"/>
-      <c r="G85" s="54"/>
-      <c r="H85" s="54"/>
-      <c r="I85" s="54"/>
-      <c r="J85" s="55"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="25"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C86" s="35" t="s">
+      <c r="C86" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="37"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="27"/>
+      <c r="H86" s="27"/>
+      <c r="I86" s="27"/>
+      <c r="J86" s="28"/>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C87" s="23" t="s">
+      <c r="C87" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
-      <c r="I87" s="24"/>
-      <c r="J87" s="25"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="30"/>
+      <c r="J87" s="31"/>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C88" s="23" t="s">
+      <c r="C88" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
-      <c r="H88" s="24"/>
-      <c r="I88" s="24"/>
-      <c r="J88" s="25"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="30"/>
+      <c r="F88" s="30"/>
+      <c r="G88" s="30"/>
+      <c r="H88" s="30"/>
+      <c r="I88" s="30"/>
+      <c r="J88" s="31"/>
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C89" s="26" t="s">
+      <c r="C89" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="28"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="34"/>
+      <c r="G89" s="34"/>
+      <c r="H89" s="34"/>
+      <c r="I89" s="34"/>
+      <c r="J89" s="35"/>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C90" s="21"/>
@@ -2441,146 +2455,99 @@
       <c r="J91" s="18"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C92" s="50" t="s">
+      <c r="C92" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="51"/>
-      <c r="E92" s="51"/>
-      <c r="F92" s="51"/>
-      <c r="G92" s="51"/>
-      <c r="H92" s="51"/>
-      <c r="I92" s="51"/>
-      <c r="J92" s="52"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="38"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C93" s="53" t="s">
+      <c r="C93" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="54"/>
-      <c r="I93" s="54"/>
-      <c r="J93" s="55"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="25"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C94" s="53" t="s">
+      <c r="C94" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D94" s="54"/>
-      <c r="E94" s="54"/>
-      <c r="F94" s="54"/>
-      <c r="G94" s="54"/>
-      <c r="H94" s="54"/>
-      <c r="I94" s="54"/>
-      <c r="J94" s="55"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="25"/>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C95" s="57" t="s">
+      <c r="C95" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="37"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="27"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="28"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C96" s="56" t="s">
+      <c r="C96" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
-      <c r="I96" s="24"/>
-      <c r="J96" s="25"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="30"/>
+      <c r="G96" s="30"/>
+      <c r="H96" s="30"/>
+      <c r="I96" s="30"/>
+      <c r="J96" s="31"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C97" s="23" t="s">
+      <c r="C97" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
-      <c r="H97" s="24"/>
-      <c r="I97" s="24"/>
-      <c r="J97" s="25"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="30"/>
+      <c r="G97" s="30"/>
+      <c r="H97" s="30"/>
+      <c r="I97" s="30"/>
+      <c r="J97" s="31"/>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C98" s="26" t="s">
+      <c r="C98" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="28"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+      <c r="I98" s="34"/>
+      <c r="J98" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="C94:J94"/>
-    <mergeCell ref="C95:J95"/>
-    <mergeCell ref="C96:J96"/>
-    <mergeCell ref="C97:J97"/>
-    <mergeCell ref="C98:J98"/>
-    <mergeCell ref="C87:J87"/>
-    <mergeCell ref="C88:J88"/>
-    <mergeCell ref="C89:J89"/>
-    <mergeCell ref="C92:J92"/>
-    <mergeCell ref="C93:J93"/>
-    <mergeCell ref="C80:J80"/>
-    <mergeCell ref="C83:J83"/>
-    <mergeCell ref="C84:J84"/>
-    <mergeCell ref="C85:J85"/>
-    <mergeCell ref="C86:J86"/>
-    <mergeCell ref="C75:J75"/>
-    <mergeCell ref="C76:J76"/>
-    <mergeCell ref="C77:J77"/>
-    <mergeCell ref="C78:J78"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="C69:J69"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="C71:J71"/>
-    <mergeCell ref="C74:J74"/>
-    <mergeCell ref="C61:J61"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="C65:J65"/>
-    <mergeCell ref="C66:J66"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C58:J58"/>
-    <mergeCell ref="C59:J59"/>
-    <mergeCell ref="C60:J60"/>
-    <mergeCell ref="C49:J49"/>
-    <mergeCell ref="C50:J50"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C53:J53"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:J48"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="C38:J38"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="C16:D16"/>
@@ -2589,14 +2556,61 @@
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="O10:Q10"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="C49:J49"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C56:J56"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C58:J58"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="C61:J61"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="C69:J69"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="C71:J71"/>
+    <mergeCell ref="C74:J74"/>
+    <mergeCell ref="C75:J75"/>
+    <mergeCell ref="C76:J76"/>
+    <mergeCell ref="C77:J77"/>
+    <mergeCell ref="C78:J78"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C80:J80"/>
+    <mergeCell ref="C83:J83"/>
+    <mergeCell ref="C84:J84"/>
+    <mergeCell ref="C85:J85"/>
+    <mergeCell ref="C86:J86"/>
+    <mergeCell ref="C87:J87"/>
+    <mergeCell ref="C88:J88"/>
+    <mergeCell ref="C89:J89"/>
+    <mergeCell ref="C92:J92"/>
+    <mergeCell ref="C93:J93"/>
+    <mergeCell ref="C94:J94"/>
+    <mergeCell ref="C95:J95"/>
+    <mergeCell ref="C96:J96"/>
+    <mergeCell ref="C97:J97"/>
+    <mergeCell ref="C98:J98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>